<commit_message>
Experiments: different learning rates for SVI
</commit_message>
<xml_diff>
--- a/extensions/lda/doc-Experiments/ResultsAbstracts.xlsx
+++ b/extensions/lda/doc-Experiments/ResultsAbstracts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="25040" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="graph" sheetId="3" r:id="rId1"/>
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>VMP_LDA</t>
   </si>
   <si>
-    <t>SVI_LDA</t>
+    <t>SVI_LDA 0.75</t>
+  </si>
+  <si>
+    <t>SVI_LDA 0.55</t>
+  </si>
+  <si>
+    <t>SVI_LDA 0.99</t>
   </si>
 </sst>
 </file>
@@ -74,8 +80,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -87,13 +97,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,7 +694,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SVI_LDA</c:v>
+                  <c:v>SVI_LDA 0.75</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1215,6 +1229,1298 @@
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>-8.89595617342651E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVI_LDA 0.55</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>29.772885355</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116.210613025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>196.451749337</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>275.664490376</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>355.355703591</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>436.354876083</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>516.3379279219999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>595.500105776</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>675.733706414</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>755.3062333189999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>835.377343309</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>917.391414495</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>997.329422294</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1077.388441828</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1157.33531572</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1237.576735715</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1316.58479572</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1395.67410451</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1474.300565238</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1553.517475194</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1633.353855366</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1712.901118926</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1792.520984042</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1872.369170303</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1953.113301943</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2033.583785039</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2112.322307065</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2191.88040956</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2272.068376397</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2351.848903708</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2431.323421029</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2510.138412459</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2590.819187926</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2671.630657701</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2751.996882495</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2831.833753528</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2911.624012622</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2990.88219625</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3073.1299319</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3153.333514655</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3233.297521183</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3313.667160166</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3393.353399907</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3473.831969229</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3554.551089894</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3635.312911904</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3717.911851213</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3797.537371968</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3877.891475835</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3958.775114776</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4038.578809084</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4118.685834026</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4200.871986324</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4282.005102424</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4361.365817457</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4441.568822658</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4524.623379412</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4603.553562304</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4683.363810881</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4763.689786503</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4844.510971128</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4924.649814645</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5004.709369907</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5085.771728744</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5165.726650851</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5246.844874606</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5327.104741478</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5407.144199171</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5488.912325711</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5569.272540012</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5649.465869251</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5729.641354027</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5810.399804048</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5890.470607949</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5969.943359863</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6049.738964374</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6130.180023674</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6210.336765768</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6290.392734204</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6371.032931651</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6452.225990414</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6531.958781334</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6611.601471797</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6692.814519619</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6773.197932437</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6852.958395219</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6935.346836886</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7014.870331524</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>7098.762754762</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7179.97562718</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>7259.550637139</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>7342.4204928</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>7422.231689521</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>7501.286616782</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>7581.083001426</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7661.336061749</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>7741.911297425</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>7823.310291159</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>7903.627994844</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>7983.326308879</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>8063.832338888</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>8144.118869487</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$103</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>-3.54530755305797E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.34161593577565E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.14741496626394E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.07292219351131E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.03011370750583E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.00731693468507E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9.933465738543E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.81283537911782E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9.71650867479247E7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.61764227974255E7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-9.53989588769068E7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-9.48338570085106E7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-9.44345403259715E7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-9.39960695856235E7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-9.36185997491749E7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-9.34131521170782E7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-9.30766418329567E7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-9.28764485725586E7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-9.26727835592623E7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-9.23355298541245E7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-9.21621364371958E7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-9.20325284436265E7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-9.18238344783423E7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-9.16859867475595E7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-9.15770343461341E7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-9.14262854435261E7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-9.13564697295345E7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-9.12969749725707E7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-9.12508390198125E7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-9.11461174579536E7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-9.10737895559735E7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-9.10344842368888E7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-9.09869008560784E7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-9.09032219020923E7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-9.07979705649484E7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-9.07404300720994E7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-9.07162861678386E7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-9.06666665719802E7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-9.06054243434195E7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-9.05707393046274E7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-9.05193693212396E7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-9.046561363135E7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-9.03903419256522E7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-9.03254698622972E7</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-9.02941987658341E7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-9.02652795107801E7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-9.01995870611363E7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-9.01508405193382E7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-9.01347495200387E7</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-9.00979594116203E7</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-9.00724486038147E7</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-8.99985260467944E7</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-8.99522390590987E7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-8.9900115139134E7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-8.98917836075356E7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-8.98833038390388E7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-8.9846062543305E7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-8.98391415775937E7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-8.98259607743574E7</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-8.97802023949223E7</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-8.97516526954717E7</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-8.97194593816301E7</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-8.9713613509914E7</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-8.96845189719676E7</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-8.96618905363919E7</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-8.96540682165429E7</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-8.96247963609622E7</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-8.96212476645941E7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-8.96394213366333E7</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-8.96111900935212E7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-8.96026652848132E7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-8.95813509856446E7</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-8.95768218724677E7</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-8.95673227869256E7</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-8.95637068731966E7</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-8.95270581554774E7</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-8.9501991026589E7</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-8.94648194788878E7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-8.94494832456695E7</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-8.94589195359648E7</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-8.94497280582214E7</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-8.94410469052061E7</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-8.94366670427806E7</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-8.9398509497464E7</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-8.93855146585406E7</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-8.93724264245984E7</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-8.93404360958437E7</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-8.93324494948712E7</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-8.93190537276624E7</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-8.93080239573073E7</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-8.93175709447E7</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-8.92895208729582E7</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-8.92928398592868E7</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-8.92812946788572E7</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-8.92606803813434E7</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-8.92705296037672E7</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-8.92629336533039E7</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-8.92540509075151E7</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-8.92468900601017E7</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-8.92335450907291E7</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-8.92152499787797E7</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-8.9205359270426E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVI_LDA 0.99</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>30.324722785</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117.661186624</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197.022218842</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>274.899156674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>353.827935097</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>432.544637832</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>510.689313053</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>588.427483853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>666.27727926</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>744.7229289650001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>822.272955819</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>899.327556721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>977.257704014</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1054.622586333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1133.602877487</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1212.000338152</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1290.196389172</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1368.084262524</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1445.887607041</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1524.806038742</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1603.415292129</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1681.046553395</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1759.878816254</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1836.935331147</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1914.8494393</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1993.286197881</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2071.125004091</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2150.009245397</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2227.258873701</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2306.093628221</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2384.006816811</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2462.83441245</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2540.897011312</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2618.92465744</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2697.4655301</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2775.532013948</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2852.791794193</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2931.110602729</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3009.201753067</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3087.282781682</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3166.292670884</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3244.620502642</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3322.487296963</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3400.577243432</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3480.144211864</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3558.066463553</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3637.079038623</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3714.866054234</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3792.674053935</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3871.980646794</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3952.566298252</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4030.500085594</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4111.343527685</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4189.712432987</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4267.767049309</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4345.657142498</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4424.077196965</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4502.030185727</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4580.31586713</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4658.608852929</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4736.285220579</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4814.195656048</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4892.080679307</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4971.770412149</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5050.53947303</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5129.031508797</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5206.976622093</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5285.045244251</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5363.083919745</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5443.082384263</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5521.927979609</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5600.331886613</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5678.278719616</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5755.496751441</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5834.026647466</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5912.148200926</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5991.476431528</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6068.530528278</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6146.809717232</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6225.213426876</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6303.635487613</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6383.230971597</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6461.889342164</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6540.36871095</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6618.004880181</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6697.327835171</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6776.451580705</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6854.611825198</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6933.473027486</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7012.602106804</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>7090.707318101</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>7169.094041155</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>7248.50345047</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>7328.467117292</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>7407.193579174</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7486.681714813</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>7565.544459188</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>7645.356434038</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>7724.674337788</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>7804.693117546</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>7883.902794804</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>7961.687431949</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$103</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>-3.68744464316883E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.36892402817465E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.14936140106248E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.07595726400032E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.03907353692047E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.01009262027948E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9.91870707112285E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.77470072007305E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9.67863363777304E7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.59836505928852E7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-9.52336860128355E7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-9.47426459106757E7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-9.43529633772391E7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-9.38747522832996E7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-9.3524677991117E7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-9.3250670040983E7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-9.2989827237754E7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-9.27828318280059E7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-9.25345119350229E7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-9.23520254979713E7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-9.21912995161269E7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-9.20843387524586E7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-9.19559389720274E7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-9.18425669746713E7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-9.17673260522429E7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-9.16943778467258E7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-9.16032579381189E7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-9.15225467963483E7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-9.14524291155844E7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-9.13438970295688E7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-9.12783927273473E7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-9.12217878407512E7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-9.11658437370924E7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-9.11001912874021E7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-9.10578687965498E7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-9.10089860154513E7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-9.09731798560863E7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-9.09309340040866E7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-9.08911426443279E7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-9.08596013944449E7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-9.08291679266149E7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-9.07977914974357E7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-9.07684024330197E7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-9.07288434744439E7</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-9.07103104216438E7</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-9.06784983056271E7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-9.06656006783614E7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-9.06443419030768E7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-9.0631037126476E7</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-9.06086334595291E7</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-9.05855581307323E7</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-9.05659768790727E7</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-9.0545120706356E7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-9.05222031742632E7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-9.05074926732318E7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-9.04956139707882E7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-9.04821470083925E7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-9.04689569173838E7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-9.04415292966737E7</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-9.0428173743778E7</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-9.04085160737392E7</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-9.03899511226434E7</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-9.03794756456981E7</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-9.03682947336243E7</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-9.03569757103217E7</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-9.03372814514655E7</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-9.03288129253586E7</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-9.0315897377173E7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-9.03037684106925E7</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-9.02923310197038E7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-9.02702773903731E7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-9.02640767322806E7</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-9.02496460067296E7</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-9.02339452704515E7</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-9.02132023983398E7</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-9.02051712955203E7</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-9.01914944500688E7</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-9.01799451291437E7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-9.01718560735318E7</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-9.01636424666905E7</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-9.01423698893878E7</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-9.01368317380217E7</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-9.01293822103503E7</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-9.01228757004359E7</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-9.01045002336392E7</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-9.00950687875873E7</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-9.0082489108951E7</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-9.00754430435154E7</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-9.00586688785877E7</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-9.00488625847546E7</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-9.00324632067406E7</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-9.00262566175031E7</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-9.00173300106894E7</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-9.00124972250052E7</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-9.00064773019809E7</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-9.0000952591419E7</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-8.99968403440705E7</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-8.99814821173775E7</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-8.99760773921893E7</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-8.99708111840638E7</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-8.99628411483911E7</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-8.99527380375216E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1229,11 +2535,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142662200"/>
-        <c:axId val="2142669512"/>
+        <c:axId val="2123170392"/>
+        <c:axId val="2123173496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142662200"/>
+        <c:axId val="2123170392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,12 +2549,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142669512"/>
+        <c:crossAx val="2123173496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142669512"/>
+        <c:axId val="2123173496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1.0E8"/>
@@ -1260,7 +2566,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142662200"/>
+        <c:crossAx val="2123170392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1281,7 +2587,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="152" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1637,15 +2943,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1655,8 +2961,14 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>489.38770924800002</v>
       </c>
@@ -1669,8 +2981,20 @@
       <c r="D2" s="1">
         <v>-358343264.97968298</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>29.772885355</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-354530755.30579698</v>
+      </c>
+      <c r="G2">
+        <v>30.324722784999999</v>
+      </c>
+      <c r="H2" s="1">
+        <v>-368744464.31688303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>574.97221974000001</v>
       </c>
@@ -1683,8 +3007,20 @@
       <c r="D3" s="1">
         <v>-134612331.21158299</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>116.210613025</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-134161593.577565</v>
+      </c>
+      <c r="G3">
+        <v>117.661186624</v>
+      </c>
+      <c r="H3" s="1">
+        <v>-136892402.81746501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>657.56530765599996</v>
       </c>
@@ -1697,8 +3033,20 @@
       <c r="D4" s="1">
         <v>-114668737.298537</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>196.451749337</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-114741496.626394</v>
+      </c>
+      <c r="G4">
+        <v>197.022218842</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-114936140.10624801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>746.92862327099999</v>
       </c>
@@ -1711,8 +3059,20 @@
       <c r="D5" s="1">
         <v>-106988533.209618</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>275.664490376</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-107292219.35113101</v>
+      </c>
+      <c r="G5">
+        <v>274.89915667399998</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-107595726.400032</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>833.19258672499996</v>
       </c>
@@ -1725,8 +3085,20 @@
       <c r="D6" s="1">
         <v>-102869588.83293501</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>355.35570359100001</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-103011370.75058299</v>
+      </c>
+      <c r="G6">
+        <v>353.82793509700002</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-103907353.692047</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>916.30727384299996</v>
       </c>
@@ -1739,8 +3111,20 @@
       <c r="D7" s="1">
         <v>-100122544.44927099</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>436.35487608300002</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-100731693.46850701</v>
+      </c>
+      <c r="G7">
+        <v>432.54463783199998</v>
+      </c>
+      <c r="H7" s="1">
+        <v>-101009262.02794801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>1002.1268944240001</v>
       </c>
@@ -1753,8 +3137,20 @@
       <c r="D8" s="1">
         <v>-98185173.494204998</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>516.33792792199995</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-99334657.385429993</v>
+      </c>
+      <c r="G8">
+        <v>510.68931305299998</v>
+      </c>
+      <c r="H8" s="1">
+        <v>-99187070.711228505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>1085.2085404869999</v>
       </c>
@@ -1767,8 +3163,20 @@
       <c r="D9" s="1">
         <v>-96806934.190176293</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>595.50010577600005</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-98128353.791178197</v>
+      </c>
+      <c r="G9">
+        <v>588.42748385300001</v>
+      </c>
+      <c r="H9" s="1">
+        <v>-97747007.200730503</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>1172.5195327829999</v>
       </c>
@@ -1781,8 +3189,20 @@
       <c r="D10" s="1">
         <v>-95828984.461923197</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>675.73370641400004</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-97165086.7479247</v>
+      </c>
+      <c r="G10">
+        <v>666.27727926</v>
+      </c>
+      <c r="H10" s="1">
+        <v>-96786336.377730399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>1268.1241052299999</v>
       </c>
@@ -1795,8 +3215,20 @@
       <c r="D11" s="1">
         <v>-94984917.954691902</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>755.30623331899994</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-96176422.797425494</v>
+      </c>
+      <c r="G11">
+        <v>744.72292896500005</v>
+      </c>
+      <c r="H11" s="1">
+        <v>-95983650.592885196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>1357.2999015759999</v>
       </c>
@@ -1809,8 +3241,20 @@
       <c r="D12" s="1">
         <v>-94334404.278949395</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>835.37734330900003</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-95398958.876906797</v>
+      </c>
+      <c r="G12">
+        <v>822.272955819</v>
+      </c>
+      <c r="H12" s="1">
+        <v>-95233686.012835503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>1448.4510817150001</v>
       </c>
@@ -1823,8 +3267,20 @@
       <c r="D13" s="1">
         <v>-93794627.676579699</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>917.39141449500005</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-94833857.008510605</v>
+      </c>
+      <c r="G13">
+        <v>899.32755672099995</v>
+      </c>
+      <c r="H13" s="1">
+        <v>-94742645.910675704</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>1542.155815849</v>
       </c>
@@ -1837,8 +3293,20 @@
       <c r="D14" s="1">
         <v>-93235321.270199999</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>997.32942229399998</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-94434540.325971499</v>
+      </c>
+      <c r="G14">
+        <v>977.25770401399996</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-94352963.377239093</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>1629.4336460300001</v>
       </c>
@@ -1851,8 +3319,20 @@
       <c r="D15" s="1">
         <v>-92805931.846822798</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>1077.3884418279999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-93996069.585623503</v>
+      </c>
+      <c r="G15">
+        <v>1054.6225863330001</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-93874752.283299595</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>1711.25632993</v>
       </c>
@@ -1865,8 +3345,20 @@
       <c r="D16" s="1">
         <v>-92446677.625006706</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>1157.3353157199999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-93618599.749174893</v>
+      </c>
+      <c r="G16">
+        <v>1133.6028774869999</v>
+      </c>
+      <c r="H16" s="1">
+        <v>-93524677.991117001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>1807.2944929929999</v>
       </c>
@@ -1879,8 +3371,20 @@
       <c r="D17" s="1">
         <v>-92137754.326045096</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>1237.576735715</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-93413152.1170782</v>
+      </c>
+      <c r="G17">
+        <v>1212.000338152</v>
+      </c>
+      <c r="H17" s="1">
+        <v>-93250670.040983006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>1889.3809454110001</v>
       </c>
@@ -1893,8 +3397,20 @@
       <c r="D18" s="1">
         <v>-91891521.054795995</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>1316.5847957200001</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-93076641.832956702</v>
+      </c>
+      <c r="G18">
+        <v>1290.196389172</v>
+      </c>
+      <c r="H18" s="1">
+        <v>-92989827.237754002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>1973.8726163030001</v>
       </c>
@@ -1907,8 +3423,20 @@
       <c r="D19" s="1">
         <v>-91682781.407398298</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>1395.67410451</v>
+      </c>
+      <c r="F19" s="1">
+        <v>-92876448.572558597</v>
+      </c>
+      <c r="G19">
+        <v>1368.084262524</v>
+      </c>
+      <c r="H19" s="1">
+        <v>-92782831.828005895</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>2059.099169263</v>
       </c>
@@ -1921,8 +3449,20 @@
       <c r="D20" s="1">
         <v>-91464519.033278599</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>1474.300565238</v>
+      </c>
+      <c r="F20" s="1">
+        <v>-92672783.559262305</v>
+      </c>
+      <c r="G20">
+        <v>1445.8876070409999</v>
+      </c>
+      <c r="H20" s="1">
+        <v>-92534511.935022905</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>2143.2265049779999</v>
       </c>
@@ -1935,8 +3475,20 @@
       <c r="D21" s="1">
         <v>-91325272.917425096</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>1553.5174751940001</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-92335529.854124501</v>
+      </c>
+      <c r="G21">
+        <v>1524.8060387420001</v>
+      </c>
+      <c r="H21" s="1">
+        <v>-92352025.497971296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>2227.0096393919998</v>
       </c>
@@ -1949,8 +3501,20 @@
       <c r="D22" s="1">
         <v>-91224996.446057305</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>1633.3538553660001</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-92162136.437195793</v>
+      </c>
+      <c r="G22">
+        <v>1603.4152921289999</v>
+      </c>
+      <c r="H22" s="1">
+        <v>-92191299.516126901</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>2307.7879977769999</v>
       </c>
@@ -1963,8 +3527,20 @@
       <c r="D23" s="1">
         <v>-91068029.234325007</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>1712.901118926</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-92032528.443626493</v>
+      </c>
+      <c r="G23">
+        <v>1681.046553395</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-92084338.752458602</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>2392.0888767370002</v>
       </c>
@@ -1977,8 +3553,20 @@
       <c r="D24" s="1">
         <v>-90934406.221337304</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>1792.520984042</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-91823834.478342295</v>
+      </c>
+      <c r="G24">
+        <v>1759.878816254</v>
+      </c>
+      <c r="H24" s="1">
+        <v>-91955938.972027406</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>2477.2810037449999</v>
       </c>
@@ -1991,8 +3579,20 @@
       <c r="D25" s="1">
         <v>-90790809.591593295</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>1872.3691703029999</v>
+      </c>
+      <c r="F25" s="1">
+        <v>-91685986.747559503</v>
+      </c>
+      <c r="G25">
+        <v>1836.9353311469999</v>
+      </c>
+      <c r="H25" s="1">
+        <v>-91842566.974671304</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>2577.510111181</v>
       </c>
@@ -2005,8 +3605,20 @@
       <c r="D26" s="1">
         <v>-90722812.770707294</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>1953.1133019429999</v>
+      </c>
+      <c r="F26" s="1">
+        <v>-91577034.346134096</v>
+      </c>
+      <c r="G26">
+        <v>1914.8494393000001</v>
+      </c>
+      <c r="H26" s="1">
+        <v>-91767326.052242905</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>2661.1140253479998</v>
       </c>
@@ -2019,8 +3631,20 @@
       <c r="D27" s="1">
         <v>-90619687.183243498</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>2033.5837850390001</v>
+      </c>
+      <c r="F27" s="1">
+        <v>-91426285.443526104</v>
+      </c>
+      <c r="G27">
+        <v>1993.2861978809999</v>
+      </c>
+      <c r="H27" s="1">
+        <v>-91694377.846725807</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>2754.2989442610001</v>
       </c>
@@ -2033,8 +3657,20 @@
       <c r="D28" s="1">
         <v>-90541961.4977725</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>2112.3223070650001</v>
+      </c>
+      <c r="F28" s="1">
+        <v>-91356469.729534507</v>
+      </c>
+      <c r="G28">
+        <v>2071.1250040909999</v>
+      </c>
+      <c r="H28" s="1">
+        <v>-91603257.938118905</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>2841.6012016630002</v>
       </c>
@@ -2047,8 +3683,20 @@
       <c r="D29" s="1">
         <v>-90453009.645570099</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>2191.8804095599999</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-91296974.972570702</v>
+      </c>
+      <c r="G29">
+        <v>2150.0092453970001</v>
+      </c>
+      <c r="H29" s="1">
+        <v>-91522546.796348304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>2933.892744453</v>
       </c>
@@ -2061,8 +3709,20 @@
       <c r="D30" s="1">
         <v>-90378144.362625495</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>2272.0683763970001</v>
+      </c>
+      <c r="F30" s="1">
+        <v>-91250839.019812495</v>
+      </c>
+      <c r="G30">
+        <v>2227.2588737010001</v>
+      </c>
+      <c r="H30" s="1">
+        <v>-91452429.115584403</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>3014.9120306929999</v>
       </c>
@@ -2075,8 +3735,20 @@
       <c r="D31" s="1">
         <v>-90296192.791279703</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>2351.8489037079999</v>
+      </c>
+      <c r="F31" s="1">
+        <v>-91146117.457953602</v>
+      </c>
+      <c r="G31">
+        <v>2306.093628221</v>
+      </c>
+      <c r="H31" s="1">
+        <v>-91343897.029568806</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>3101.3842716140002</v>
       </c>
@@ -2089,8 +3761,20 @@
       <c r="D32" s="1">
         <v>-90225073.929240301</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>2431.3234210290002</v>
+      </c>
+      <c r="F32" s="1">
+        <v>-91073789.5559735</v>
+      </c>
+      <c r="G32">
+        <v>2384.0068168110001</v>
+      </c>
+      <c r="H32" s="1">
+        <v>-91278392.727347299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>3183.747145496</v>
       </c>
@@ -2103,8 +3787,20 @@
       <c r="D33" s="1">
         <v>-90127805.302648798</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>2510.1384124589999</v>
+      </c>
+      <c r="F33" s="1">
+        <v>-91034484.236888796</v>
+      </c>
+      <c r="G33">
+        <v>2462.8344124499999</v>
+      </c>
+      <c r="H33" s="1">
+        <v>-91221787.840751201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>3280.1833212890001</v>
       </c>
@@ -2117,8 +3813,20 @@
       <c r="D34" s="1">
         <v>-90064988.044430301</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>2590.8191879259998</v>
+      </c>
+      <c r="F34" s="1">
+        <v>-90986900.856078401</v>
+      </c>
+      <c r="G34">
+        <v>2540.8970113119999</v>
+      </c>
+      <c r="H34" s="1">
+        <v>-91165843.737092406</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>3370.9487138690001</v>
       </c>
@@ -2131,8 +3839,20 @@
       <c r="D35" s="1">
         <v>-90005197.509552404</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>2671.630657701</v>
+      </c>
+      <c r="F35" s="1">
+        <v>-90903221.902092293</v>
+      </c>
+      <c r="G35">
+        <v>2618.9246574399999</v>
+      </c>
+      <c r="H35" s="1">
+        <v>-91100191.287402093</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>3452.503192618</v>
       </c>
@@ -2145,8 +3865,20 @@
       <c r="D36" s="1">
         <v>-89972435.749769598</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>2751.9968824950001</v>
+      </c>
+      <c r="F36" s="1">
+        <v>-90797970.564948395</v>
+      </c>
+      <c r="G36">
+        <v>2697.4655300999998</v>
+      </c>
+      <c r="H36" s="1">
+        <v>-91057868.796549797</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>3541.9968423959999</v>
       </c>
@@ -2159,8 +3891,20 @@
       <c r="D37" s="1">
         <v>-89922927.205974698</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>2831.8337535280002</v>
+      </c>
+      <c r="F37" s="1">
+        <v>-90740430.072099403</v>
+      </c>
+      <c r="G37">
+        <v>2775.532013948</v>
+      </c>
+      <c r="H37" s="1">
+        <v>-91008986.015451297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>3628.055724672</v>
       </c>
@@ -2173,8 +3917,20 @@
       <c r="D38" s="1">
         <v>-89881429.227250904</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>2911.624012622</v>
+      </c>
+      <c r="F38" s="1">
+        <v>-90716286.167838603</v>
+      </c>
+      <c r="G38">
+        <v>2852.791794193</v>
+      </c>
+      <c r="H38" s="1">
+        <v>-90973179.856086299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>3708.613198728</v>
       </c>
@@ -2187,8 +3943,20 @@
       <c r="D39" s="1">
         <v>-89806965.350713804</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>2990.8821962500001</v>
+      </c>
+      <c r="F39" s="1">
+        <v>-90666666.571980193</v>
+      </c>
+      <c r="G39">
+        <v>2931.1106027290002</v>
+      </c>
+      <c r="H39" s="1">
+        <v>-90930934.004086599</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>3794.4533790199998</v>
       </c>
@@ -2201,8 +3969,20 @@
       <c r="D40" s="1">
         <v>-89775263.179527506</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>3073.1299319</v>
+      </c>
+      <c r="F40" s="1">
+        <v>-90605424.343419507</v>
+      </c>
+      <c r="G40">
+        <v>3009.201753067</v>
+      </c>
+      <c r="H40" s="1">
+        <v>-90891142.644327894</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>3877.9043087939999</v>
       </c>
@@ -2215,8 +3995,20 @@
       <c r="D41" s="1">
         <v>-89745287.460990399</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>3153.3335146549998</v>
+      </c>
+      <c r="F41" s="1">
+        <v>-90570739.304627404</v>
+      </c>
+      <c r="G41">
+        <v>3087.2827816819999</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-90859601.394444898</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>3965.3343505319999</v>
       </c>
@@ -2229,8 +4021,20 @@
       <c r="D42" s="1">
         <v>-89706485.758113101</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42">
+        <v>3233.2975211829998</v>
+      </c>
+      <c r="F42" s="1">
+        <v>-90519369.321239606</v>
+      </c>
+      <c r="G42">
+        <v>3166.292670884</v>
+      </c>
+      <c r="H42" s="1">
+        <v>-90829167.926614895</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>4053.2819607910001</v>
       </c>
@@ -2243,8 +4047,20 @@
       <c r="D43" s="1">
         <v>-89679214.4465684</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <v>3313.667160166</v>
+      </c>
+      <c r="F43" s="1">
+        <v>-90465613.631349996</v>
+      </c>
+      <c r="G43">
+        <v>3244.6205026419998</v>
+      </c>
+      <c r="H43" s="1">
+        <v>-90797791.497435704</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>4138.1563136840005</v>
       </c>
@@ -2257,8 +4073,20 @@
       <c r="D44" s="1">
         <v>-89622773.572599307</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44">
+        <v>3393.353399907</v>
+      </c>
+      <c r="F44" s="1">
+        <v>-90390341.925652206</v>
+      </c>
+      <c r="G44">
+        <v>3322.4872969630001</v>
+      </c>
+      <c r="H44" s="1">
+        <v>-90768402.433019698</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>4224.0407658149998</v>
       </c>
@@ -2271,8 +4099,20 @@
       <c r="D45" s="1">
         <v>-89595294.449494302</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45">
+        <v>3473.8319692290002</v>
+      </c>
+      <c r="F45" s="1">
+        <v>-90325469.862297207</v>
+      </c>
+      <c r="G45">
+        <v>3400.5772434320002</v>
+      </c>
+      <c r="H45" s="1">
+        <v>-90728843.474443898</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>4308.1737339789997</v>
       </c>
@@ -2285,8 +4125,20 @@
       <c r="D46" s="1">
         <v>-89560912.284912795</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46">
+        <v>3554.5510898940001</v>
+      </c>
+      <c r="F46" s="1">
+        <v>-90294198.765834093</v>
+      </c>
+      <c r="G46">
+        <v>3480.1442118640002</v>
+      </c>
+      <c r="H46" s="1">
+        <v>-90710310.421643794</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>4387.870082425</v>
       </c>
@@ -2299,8 +4151,20 @@
       <c r="D47" s="1">
         <v>-89535254.313057199</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47">
+        <v>3635.312911904</v>
+      </c>
+      <c r="F47" s="1">
+        <v>-90265279.510780096</v>
+      </c>
+      <c r="G47">
+        <v>3558.0664635530002</v>
+      </c>
+      <c r="H47" s="1">
+        <v>-90678498.305627093</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>4472.2596474559996</v>
       </c>
@@ -2313,8 +4177,20 @@
       <c r="D48" s="1">
         <v>-89502575.559397101</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48">
+        <v>3717.9118512129999</v>
+      </c>
+      <c r="F48" s="1">
+        <v>-90199587.061136305</v>
+      </c>
+      <c r="G48">
+        <v>3637.0790386230001</v>
+      </c>
+      <c r="H48" s="1">
+        <v>-90665600.678361401</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>4559.5062242169997</v>
       </c>
@@ -2327,8 +4203,20 @@
       <c r="D49" s="1">
         <v>-89466759.080936</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49">
+        <v>3797.5373719680001</v>
+      </c>
+      <c r="F49" s="1">
+        <v>-90150840.519338205</v>
+      </c>
+      <c r="G49">
+        <v>3714.8660542339999</v>
+      </c>
+      <c r="H49" s="1">
+        <v>-90644341.903076798</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>4640.9443851409997</v>
       </c>
@@ -2341,8 +4229,20 @@
       <c r="D50" s="1">
         <v>-89441227.598258898</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50">
+        <v>3877.8914758350002</v>
+      </c>
+      <c r="F50" s="1">
+        <v>-90134749.520038694</v>
+      </c>
+      <c r="G50">
+        <v>3792.6740539349998</v>
+      </c>
+      <c r="H50" s="1">
+        <v>-90631037.1264759</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>4722.9760108230003</v>
       </c>
@@ -2355,8 +4255,20 @@
       <c r="D51" s="1">
         <v>-89412005.964233994</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51">
+        <v>3958.775114776</v>
+      </c>
+      <c r="F51" s="1">
+        <v>-90097959.411620304</v>
+      </c>
+      <c r="G51">
+        <v>3871.9806467940002</v>
+      </c>
+      <c r="H51" s="1">
+        <v>-90608633.459529102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>4807.477013572</v>
       </c>
@@ -2369,8 +4281,20 @@
       <c r="D52" s="1">
         <v>-89385986.774235398</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <v>4038.5788090840001</v>
+      </c>
+      <c r="F52" s="1">
+        <v>-90072448.603814706</v>
+      </c>
+      <c r="G52">
+        <v>3952.5662982519998</v>
+      </c>
+      <c r="H52" s="1">
+        <v>-90585558.130732298</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>4900.736318583</v>
       </c>
@@ -2383,8 +4307,20 @@
       <c r="D53" s="1">
         <v>-89366099.854775906</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <v>4118.6858340259996</v>
+      </c>
+      <c r="F53" s="1">
+        <v>-89998526.0467944</v>
+      </c>
+      <c r="G53">
+        <v>4030.5000855940002</v>
+      </c>
+      <c r="H53" s="1">
+        <v>-90565976.879072696</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>4993.7933120409998</v>
       </c>
@@ -2397,8 +4333,20 @@
       <c r="D54" s="1">
         <v>-89349052.654121205</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <v>4200.8719863240003</v>
+      </c>
+      <c r="F54" s="1">
+        <v>-89952239.059098706</v>
+      </c>
+      <c r="G54">
+        <v>4111.3435276849996</v>
+      </c>
+      <c r="H54" s="1">
+        <v>-90545120.706356004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>5077.3153561790004</v>
       </c>
@@ -2411,8 +4359,20 @@
       <c r="D55" s="1">
         <v>-89329325.817590594</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55">
+        <v>4282.0051024240001</v>
+      </c>
+      <c r="F55" s="1">
+        <v>-89900115.1391339</v>
+      </c>
+      <c r="G55">
+        <v>4189.7124329870003</v>
+      </c>
+      <c r="H55" s="1">
+        <v>-90522203.174263194</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>5167.2838674220002</v>
       </c>
@@ -2425,8 +4385,20 @@
       <c r="D56" s="1">
         <v>-89307847.253371701</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56">
+        <v>4361.365817457</v>
+      </c>
+      <c r="F56" s="1">
+        <v>-89891783.607535601</v>
+      </c>
+      <c r="G56">
+        <v>4267.767049309</v>
+      </c>
+      <c r="H56" s="1">
+        <v>-90507492.673231795</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>5248.1468279740002</v>
       </c>
@@ -2439,8 +4411,20 @@
       <c r="D57" s="1">
         <v>-89298718.9456155</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57">
+        <v>4441.5688226579996</v>
+      </c>
+      <c r="F57" s="1">
+        <v>-89883303.839038804</v>
+      </c>
+      <c r="G57">
+        <v>4345.6571424980002</v>
+      </c>
+      <c r="H57" s="1">
+        <v>-90495613.970788196</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>5327.860626869</v>
       </c>
@@ -2453,8 +4437,20 @@
       <c r="D58" s="1">
         <v>-89284997.490857199</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58">
+        <v>4524.6233794119998</v>
+      </c>
+      <c r="F58" s="1">
+        <v>-89846062.543304905</v>
+      </c>
+      <c r="G58">
+        <v>4424.0771969650004</v>
+      </c>
+      <c r="H58" s="1">
+        <v>-90482147.008392498</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>5414.9418567539997</v>
       </c>
@@ -2467,8 +4463,20 @@
       <c r="D59" s="1">
         <v>-89274100.681614295</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59">
+        <v>4603.5535623039996</v>
+      </c>
+      <c r="F59" s="1">
+        <v>-89839141.577593699</v>
+      </c>
+      <c r="G59">
+        <v>4502.0301857269997</v>
+      </c>
+      <c r="H59" s="1">
+        <v>-90468956.917383805</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>5502.949690169</v>
       </c>
@@ -2481,8 +4489,20 @@
       <c r="D60" s="1">
         <v>-89256501.376148298</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60">
+        <v>4683.3638108810001</v>
+      </c>
+      <c r="F60" s="1">
+        <v>-89825960.774357393</v>
+      </c>
+      <c r="G60">
+        <v>4580.3158671299998</v>
+      </c>
+      <c r="H60" s="1">
+        <v>-90441529.2966737</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>5587.9830419580003</v>
       </c>
@@ -2495,8 +4515,20 @@
       <c r="D61" s="1">
         <v>-89248319.874739602</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61">
+        <v>4763.6897865029996</v>
+      </c>
+      <c r="F61" s="1">
+        <v>-89780202.394922301</v>
+      </c>
+      <c r="G61">
+        <v>4658.608852929</v>
+      </c>
+      <c r="H61" s="1">
+        <v>-90428173.743777901</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>5673.0332255330004</v>
       </c>
@@ -2509,8 +4541,20 @@
       <c r="D62" s="1">
         <v>-89236201.594375193</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62">
+        <v>4844.5109711280002</v>
+      </c>
+      <c r="F62" s="1">
+        <v>-89751652.695471704</v>
+      </c>
+      <c r="G62">
+        <v>4736.2852205790005</v>
+      </c>
+      <c r="H62" s="1">
+        <v>-90408516.073739201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>5763.4496364679999</v>
       </c>
@@ -2523,8 +4567,20 @@
       <c r="D63" s="1">
         <v>-89222966.428638697</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63">
+        <v>4924.6498146450003</v>
+      </c>
+      <c r="F63" s="1">
+        <v>-89719459.381630093</v>
+      </c>
+      <c r="G63">
+        <v>4814.1956560480003</v>
+      </c>
+      <c r="H63" s="1">
+        <v>-90389951.122643396</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>5850.1768772380001</v>
       </c>
@@ -2537,8 +4593,20 @@
       <c r="D64" s="1">
         <v>-89199986.197035402</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64">
+        <v>5004.7093699070001</v>
+      </c>
+      <c r="F64" s="1">
+        <v>-89713613.509913996</v>
+      </c>
+      <c r="G64">
+        <v>4892.0806793069996</v>
+      </c>
+      <c r="H64" s="1">
+        <v>-90379475.6456981</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65">
         <v>5931.870796616</v>
       </c>
@@ -2551,8 +4619,20 @@
       <c r="D65" s="1">
         <v>-89189829.996883795</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65">
+        <v>5085.771728744</v>
+      </c>
+      <c r="F65" s="1">
+        <v>-89684518.971967593</v>
+      </c>
+      <c r="G65">
+        <v>4971.7704121489996</v>
+      </c>
+      <c r="H65" s="1">
+        <v>-90368294.733624294</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66">
         <v>6014.5937229560004</v>
       </c>
@@ -2565,8 +4645,20 @@
       <c r="D66" s="1">
         <v>-89181853.959099993</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66">
+        <v>5165.7266508510002</v>
+      </c>
+      <c r="F66" s="1">
+        <v>-89661890.536391899</v>
+      </c>
+      <c r="G66">
+        <v>5050.5394730300004</v>
+      </c>
+      <c r="H66" s="1">
+        <v>-90356975.710321695</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67">
         <v>6096.2897777770004</v>
       </c>
@@ -2579,8 +4671,20 @@
       <c r="D67" s="1">
         <v>-89164322.3204633</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67">
+        <v>5246.8448746060003</v>
+      </c>
+      <c r="F67" s="1">
+        <v>-89654068.2165429</v>
+      </c>
+      <c r="G67">
+        <v>5129.0315087970002</v>
+      </c>
+      <c r="H67" s="1">
+        <v>-90337281.451465502</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68">
         <v>6185.8796873319998</v>
       </c>
@@ -2593,8 +4697,20 @@
       <c r="D68" s="1">
         <v>-89154048.618503198</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68">
+        <v>5327.1047414779996</v>
+      </c>
+      <c r="F68" s="1">
+        <v>-89624796.360962197</v>
+      </c>
+      <c r="G68">
+        <v>5206.9766220929996</v>
+      </c>
+      <c r="H68" s="1">
+        <v>-90328812.925358593</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69">
         <v>6276.3603512959999</v>
       </c>
@@ -2607,8 +4723,20 @@
       <c r="D69" s="1">
         <v>-89148601.530194893</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69">
+        <v>5407.1441991709999</v>
+      </c>
+      <c r="F69" s="1">
+        <v>-89621247.664594099</v>
+      </c>
+      <c r="G69">
+        <v>5285.0452442510004</v>
+      </c>
+      <c r="H69" s="1">
+        <v>-90315897.377173007</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70">
         <v>6358.0639332979999</v>
       </c>
@@ -2621,8 +4749,20 @@
       <c r="D70" s="1">
         <v>-89123317.041192502</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70">
+        <v>5488.9123257110004</v>
+      </c>
+      <c r="F70" s="1">
+        <v>-89639421.336633295</v>
+      </c>
+      <c r="G70">
+        <v>5363.0839197449995</v>
+      </c>
+      <c r="H70" s="1">
+        <v>-90303768.410692498</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71">
         <v>6441.0701698379999</v>
       </c>
@@ -2635,8 +4775,20 @@
       <c r="D71" s="1">
         <v>-89112703.330711201</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71">
+        <v>5569.2725400119998</v>
+      </c>
+      <c r="F71" s="1">
+        <v>-89611190.093521193</v>
+      </c>
+      <c r="G71">
+        <v>5443.0823842629998</v>
+      </c>
+      <c r="H71" s="1">
+        <v>-90292331.019703805</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72">
         <v>6523.9539932910002</v>
       </c>
@@ -2649,8 +4801,20 @@
       <c r="D72" s="1">
         <v>-89099003.4332757</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72">
+        <v>5649.4658692510002</v>
+      </c>
+      <c r="F72" s="1">
+        <v>-89602665.284813195</v>
+      </c>
+      <c r="G72">
+        <v>5521.9279796090004</v>
+      </c>
+      <c r="H72" s="1">
+        <v>-90270277.390373096</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73">
         <v>6614.2454261760004</v>
       </c>
@@ -2663,8 +4827,20 @@
       <c r="D73" s="1">
         <v>-89084302.106438205</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73">
+        <v>5729.6413540269996</v>
+      </c>
+      <c r="F73" s="1">
+        <v>-89581350.985644594</v>
+      </c>
+      <c r="G73">
+        <v>5600.3318866130003</v>
+      </c>
+      <c r="H73" s="1">
+        <v>-90264076.732280597</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74">
         <v>6704.1278316850003</v>
       </c>
@@ -2677,8 +4853,20 @@
       <c r="D74" s="1">
         <v>-89071039.515169993</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74">
+        <v>5810.3998040480001</v>
+      </c>
+      <c r="F74" s="1">
+        <v>-89576821.872467697</v>
+      </c>
+      <c r="G74">
+        <v>5678.2787196159998</v>
+      </c>
+      <c r="H74" s="1">
+        <v>-90249646.006729603</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75">
         <v>6788.4592326749998</v>
       </c>
@@ -2691,8 +4879,20 @@
       <c r="D75" s="1">
         <v>-89059037.592787504</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75">
+        <v>5890.4706079489997</v>
+      </c>
+      <c r="F75" s="1">
+        <v>-89567322.786925599</v>
+      </c>
+      <c r="G75">
+        <v>5755.496751441</v>
+      </c>
+      <c r="H75" s="1">
+        <v>-90233945.270451501</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76">
         <v>6868.820898076</v>
       </c>
@@ -2705,8 +4905,20 @@
       <c r="D76" s="1">
         <v>-89052807.103436098</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76">
+        <v>5969.9433598630003</v>
+      </c>
+      <c r="F76" s="1">
+        <v>-89563706.873196602</v>
+      </c>
+      <c r="G76">
+        <v>5834.0266474660002</v>
+      </c>
+      <c r="H76" s="1">
+        <v>-90213202.398339793</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77">
         <v>6952.1703167129999</v>
       </c>
@@ -2719,8 +4931,20 @@
       <c r="D77" s="1">
         <v>-89041325.169960707</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77">
+        <v>6049.7389643739998</v>
+      </c>
+      <c r="F77" s="1">
+        <v>-89527058.155477405</v>
+      </c>
+      <c r="G77">
+        <v>5912.1482009259998</v>
+      </c>
+      <c r="H77" s="1">
+        <v>-90205171.295520306</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78">
         <v>7036.8318155340003</v>
       </c>
@@ -2733,8 +4957,20 @@
       <c r="D78" s="1">
         <v>-89031558.398013905</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78">
+        <v>6130.180023674</v>
+      </c>
+      <c r="F78" s="1">
+        <v>-89501991.026588902</v>
+      </c>
+      <c r="G78">
+        <v>5991.4764315279999</v>
+      </c>
+      <c r="H78" s="1">
+        <v>-90191494.450068802</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79">
         <v>7129.2066762300001</v>
       </c>
@@ -2747,8 +4983,20 @@
       <c r="D79" s="1">
         <v>-89021680.830824301</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79">
+        <v>6210.3367657680001</v>
+      </c>
+      <c r="F79" s="1">
+        <v>-89464819.478887796</v>
+      </c>
+      <c r="G79">
+        <v>6068.530528278</v>
+      </c>
+      <c r="H79" s="1">
+        <v>-90179945.1291437</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80">
         <v>7213.3564373440004</v>
       </c>
@@ -2761,8 +5009,20 @@
       <c r="D80" s="1">
         <v>-89008421.352423295</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80">
+        <v>6290.3927342039997</v>
+      </c>
+      <c r="F80" s="1">
+        <v>-89449483.245669499</v>
+      </c>
+      <c r="G80">
+        <v>6146.8097172320004</v>
+      </c>
+      <c r="H80" s="1">
+        <v>-90171856.073531806</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81">
         <v>7295.4299291079997</v>
       </c>
@@ -2775,8 +5035,20 @@
       <c r="D81" s="1">
         <v>-88999719.741282806</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81">
+        <v>6371.0329316509997</v>
+      </c>
+      <c r="F81" s="1">
+        <v>-89458919.535964802</v>
+      </c>
+      <c r="G81">
+        <v>6225.2134268760001</v>
+      </c>
+      <c r="H81" s="1">
+        <v>-90163642.466690496</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82">
         <v>7376.8780546469998</v>
       </c>
@@ -2789,8 +5061,20 @@
       <c r="D82" s="1">
         <v>-88991512.322523594</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82">
+        <v>6452.2259904140001</v>
+      </c>
+      <c r="F82" s="1">
+        <v>-89449728.0582214</v>
+      </c>
+      <c r="G82">
+        <v>6303.6354876129999</v>
+      </c>
+      <c r="H82" s="1">
+        <v>-90142369.889387801</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83">
         <v>7463.3609744200003</v>
       </c>
@@ -2803,8 +5087,20 @@
       <c r="D83" s="1">
         <v>-88982724.680895895</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83">
+        <v>6531.9587813340004</v>
+      </c>
+      <c r="F83" s="1">
+        <v>-89441046.905206099</v>
+      </c>
+      <c r="G83">
+        <v>6383.2309715969996</v>
+      </c>
+      <c r="H83" s="1">
+        <v>-90136831.738021702</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84">
         <v>7555.1126597390003</v>
       </c>
@@ -2817,8 +5113,20 @@
       <c r="D84" s="1">
         <v>-88980502.266430303</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84">
+        <v>6611.6014717970002</v>
+      </c>
+      <c r="F84" s="1">
+        <v>-89436667.042780593</v>
+      </c>
+      <c r="G84">
+        <v>6461.8893421639996</v>
+      </c>
+      <c r="H84" s="1">
+        <v>-90129382.210350305</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85">
         <v>7643.6294753459997</v>
       </c>
@@ -2831,8 +5139,20 @@
       <c r="D85" s="1">
         <v>-88972920.126532599</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85">
+        <v>6692.8145196189998</v>
+      </c>
+      <c r="F85" s="1">
+        <v>-89398509.497464001</v>
+      </c>
+      <c r="G85">
+        <v>6540.3687109499997</v>
+      </c>
+      <c r="H85" s="1">
+        <v>-90122875.700435907</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86">
         <v>7728.5872792290002</v>
       </c>
@@ -2845,8 +5165,20 @@
       <c r="D86" s="1">
         <v>-88967907.967875406</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86">
+        <v>6773.1979324370004</v>
+      </c>
+      <c r="F86" s="1">
+        <v>-89385514.658540606</v>
+      </c>
+      <c r="G86">
+        <v>6618.0048801809999</v>
+      </c>
+      <c r="H86" s="1">
+        <v>-90104500.233639196</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87">
         <v>7813.9675419360001</v>
       </c>
@@ -2859,141 +5191,351 @@
       <c r="D87" s="1">
         <v>-88959561.734265104</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87">
+        <v>6852.9583952189996</v>
+      </c>
+      <c r="F87" s="1">
+        <v>-89372426.424598396</v>
+      </c>
+      <c r="G87">
+        <v>6697.3278351709996</v>
+      </c>
+      <c r="H87" s="1">
+        <v>-90095068.7875873</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
       <c r="C88">
         <v>7004.0263572020003</v>
       </c>
       <c r="D88" s="1">
         <v>-88943551.154164195</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88">
+        <v>6935.3468368860003</v>
+      </c>
+      <c r="F88" s="1">
+        <v>-89340436.095843703</v>
+      </c>
+      <c r="G88">
+        <v>6776.4515807050002</v>
+      </c>
+      <c r="H88" s="1">
+        <v>-90082489.108951002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
       <c r="C89">
         <v>7084.9143788669999</v>
       </c>
       <c r="D89" s="1">
         <v>-88919937.6429286</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89">
+        <v>7014.870331524</v>
+      </c>
+      <c r="F89" s="1">
+        <v>-89332449.494871199</v>
+      </c>
+      <c r="G89">
+        <v>6854.6118251979997</v>
+      </c>
+      <c r="H89" s="1">
+        <v>-90075443.043515399</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="C90">
         <v>7166.0591257349997</v>
       </c>
       <c r="D90" s="1">
         <v>-88912721.296558499</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90">
+        <v>7098.7627547620004</v>
+      </c>
+      <c r="F90" s="1">
+        <v>-89319053.727662399</v>
+      </c>
+      <c r="G90">
+        <v>6933.4730274860003</v>
+      </c>
+      <c r="H90" s="1">
+        <v>-90058668.878587693</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="C91">
         <v>7247.1632872560003</v>
       </c>
       <c r="D91" s="1">
         <v>-88909017.348965198</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91">
+        <v>7179.9756271799997</v>
+      </c>
+      <c r="F91" s="1">
+        <v>-89308023.957307294</v>
+      </c>
+      <c r="G91">
+        <v>7012.602106804</v>
+      </c>
+      <c r="H91" s="1">
+        <v>-90048862.584754601</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
       <c r="C92">
         <v>7331.1920213020003</v>
       </c>
       <c r="D92" s="1">
         <v>-88894823.297623798</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92">
+        <v>7259.5506371390002</v>
+      </c>
+      <c r="F92" s="1">
+        <v>-89317570.944700003</v>
+      </c>
+      <c r="G92">
+        <v>7090.7073181010001</v>
+      </c>
+      <c r="H92" s="1">
+        <v>-90032463.206740603</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
       <c r="C93">
         <v>7413.3144120919997</v>
       </c>
       <c r="D93" s="1">
         <v>-88886077.412701905</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93">
+        <v>7342.4204927999999</v>
+      </c>
+      <c r="F93" s="1">
+        <v>-89289520.872958198</v>
+      </c>
+      <c r="G93">
+        <v>7169.094041155</v>
+      </c>
+      <c r="H93" s="1">
+        <v>-90026256.617503107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
       <c r="C94">
         <v>7494.7410021770002</v>
       </c>
       <c r="D94" s="1">
         <v>-88882531.624963298</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94">
+        <v>7422.2316895209997</v>
+      </c>
+      <c r="F94" s="1">
+        <v>-89292839.8592868</v>
+      </c>
+      <c r="G94">
+        <v>7248.5034504699997</v>
+      </c>
+      <c r="H94" s="1">
+        <v>-90017330.010689393</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
       <c r="C95">
         <v>7575.2724799549997</v>
       </c>
       <c r="D95" s="1">
         <v>-88880582.046487004</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95">
+        <v>7501.2866167820002</v>
+      </c>
+      <c r="F95" s="1">
+        <v>-89281294.678857207</v>
+      </c>
+      <c r="G95">
+        <v>7328.4671172919998</v>
+      </c>
+      <c r="H95" s="1">
+        <v>-90012497.225005195</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
       <c r="C96">
         <v>7658.383414979</v>
       </c>
       <c r="D96" s="1">
         <v>-88875712.339835897</v>
       </c>
-    </row>
-    <row r="97" spans="3:4">
+      <c r="E96">
+        <v>7581.083001426</v>
+      </c>
+      <c r="F96" s="1">
+        <v>-89260680.381343395</v>
+      </c>
+      <c r="G96">
+        <v>7407.1935791739998</v>
+      </c>
+      <c r="H96" s="1">
+        <v>-90006477.301980898</v>
+      </c>
+    </row>
+    <row r="97" spans="3:8">
       <c r="C97">
         <v>7739.610443351</v>
       </c>
       <c r="D97" s="1">
         <v>-88864268.326571196</v>
       </c>
-    </row>
-    <row r="98" spans="3:4">
+      <c r="E97">
+        <v>7661.3360617489998</v>
+      </c>
+      <c r="F97" s="1">
+        <v>-89270529.603767201</v>
+      </c>
+      <c r="G97">
+        <v>7486.6817148130003</v>
+      </c>
+      <c r="H97" s="1">
+        <v>-90000952.591418996</v>
+      </c>
+    </row>
+    <row r="98" spans="3:8">
       <c r="C98">
         <v>7821.0055573379996</v>
       </c>
       <c r="D98" s="1">
         <v>-88857200.779608995</v>
       </c>
-    </row>
-    <row r="99" spans="3:4">
+      <c r="E98">
+        <v>7741.9112974250002</v>
+      </c>
+      <c r="F98" s="1">
+        <v>-89262933.653303906</v>
+      </c>
+      <c r="G98">
+        <v>7565.5444591879996</v>
+      </c>
+      <c r="H98" s="1">
+        <v>-89996840.344070494</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8">
       <c r="C99">
         <v>7903.5175374419996</v>
       </c>
       <c r="D99" s="1">
         <v>-88853871.805162698</v>
       </c>
-    </row>
-    <row r="100" spans="3:4">
+      <c r="E99">
+        <v>7823.3102911590004</v>
+      </c>
+      <c r="F99" s="1">
+        <v>-89254050.907515094</v>
+      </c>
+      <c r="G99">
+        <v>7645.3564340379999</v>
+      </c>
+      <c r="H99" s="1">
+        <v>-89981482.117377505</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8">
       <c r="C100">
         <v>7983.7643197150001</v>
       </c>
       <c r="D100" s="1">
         <v>-88851579.984792203</v>
       </c>
-    </row>
-    <row r="101" spans="3:4">
+      <c r="E100">
+        <v>7903.6279948439997</v>
+      </c>
+      <c r="F100" s="1">
+        <v>-89246890.060101703</v>
+      </c>
+      <c r="G100">
+        <v>7724.6743377880002</v>
+      </c>
+      <c r="H100" s="1">
+        <v>-89976077.392189294</v>
+      </c>
+    </row>
+    <row r="101" spans="3:8">
       <c r="C101">
         <v>8064.8521343809998</v>
       </c>
       <c r="D101" s="1">
         <v>-88843420.020253807</v>
       </c>
-    </row>
-    <row r="102" spans="3:4">
+      <c r="E101">
+        <v>7983.326308879</v>
+      </c>
+      <c r="F101" s="1">
+        <v>-89233545.090729102</v>
+      </c>
+      <c r="G101">
+        <v>7804.6931175460004</v>
+      </c>
+      <c r="H101" s="1">
+        <v>-89970811.184063807</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8">
       <c r="C102">
         <v>8146.9259378090001</v>
       </c>
       <c r="D102" s="1">
         <v>-88840218.861460298</v>
       </c>
-    </row>
-    <row r="103" spans="3:4">
+      <c r="E102">
+        <v>8063.8323388879999</v>
+      </c>
+      <c r="F102" s="1">
+        <v>-89215249.978779703</v>
+      </c>
+      <c r="G102">
+        <v>7883.9027948040002</v>
+      </c>
+      <c r="H102" s="1">
+        <v>-89962841.148391098</v>
+      </c>
+    </row>
+    <row r="103" spans="3:8">
       <c r="C103">
         <v>8227.1838911270006</v>
       </c>
       <c r="D103" s="1">
         <v>-88833705.826926604</v>
       </c>
-    </row>
-    <row r="104" spans="3:4">
+      <c r="E103">
+        <v>8144.1188694869998</v>
+      </c>
+      <c r="F103" s="1">
+        <v>-89205359.270426005</v>
+      </c>
+      <c r="G103">
+        <v>7961.6874319489998</v>
+      </c>
+      <c r="H103" s="1">
+        <v>-89952738.037521601</v>
+      </c>
+    </row>
+    <row r="104" spans="3:8">
       <c r="C104">
         <v>8308.2341595689995</v>
       </c>
       <c r="D104" s="1">
         <v>-88827599.848858103</v>
+      </c>
+      <c r="E104">
+        <v>8223.4484774249995</v>
+      </c>
+      <c r="F104">
+        <v>-144160.336547265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>